<commit_message>
Change template to add Date Placeholder
</commit_message>
<xml_diff>
--- a/deploy/go/TemplateOutput.xlsx
+++ b/deploy/go/TemplateOutput.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Project\Golang\JadwalPetugas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Project\nodejs\church-scheduler-electron\deploy\go\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07671EE6-B205-4B3B-99C9-3708B40D3F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FDF27B-846C-4A76-95BB-02662A17978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,126 +20,94 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>WAKTU</t>
   </si>
   <si>
-    <t>MINGGU, 03 AUGUST 2025
+    <t>DP/PA</t>
+  </si>
+  <si>
+    <t>W/PB</t>
+  </si>
+  <si>
+    <t>Persembahan</t>
+  </si>
+  <si>
+    <t>Multimedia</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>UMUM</t>
+  </si>
+  <si>
+    <t>REMAJA/PEMUDA</t>
+  </si>
+  <si>
+    <t>Majels Pendamping</t>
+  </si>
+  <si>
+    <t>Lektor 1</t>
+  </si>
+  <si>
+    <t>Lektor 2</t>
+  </si>
+  <si>
+    <t>Prokantor 1</t>
+  </si>
+  <si>
+    <t>Prokantor 2</t>
+  </si>
+  <si>
+    <t>Pemusik 1</t>
+  </si>
+  <si>
+    <t>Pemusik 2</t>
+  </si>
+  <si>
+    <t>Pemusik 3</t>
+  </si>
+  <si>
+    <t>Lektor 3</t>
+  </si>
+  <si>
+    <t>Prokantor 3</t>
+  </si>
+  <si>
+    <t>Lektor 4</t>
+  </si>
+  <si>
+    <t>P. Jemaat 1</t>
+  </si>
+  <si>
+    <t>P. Jemaat 2</t>
+  </si>
+  <si>
+    <t>P. Jemaat 3</t>
+  </si>
+  <si>
+    <t>P. Jemaat 4</t>
+  </si>
+  <si>
+    <t>Kolektan 1</t>
+  </si>
+  <si>
+    <t>Kolektan 2</t>
+  </si>
+  <si>
+    <t>Kolektan 4</t>
+  </si>
+  <si>
+    <t>Kolektan 3</t>
+  </si>
+  <si>
+    <t>{Day}, {dd} {MMM} {yyyy}
 Pkl. 07.00 Wib,</t>
   </si>
   <si>
-    <t>MINGGU, 10 AUGUST 2025
-Pkl. 07.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 17 AUGUST 2025
-Pkl. 07.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 24 AUGUST 2025
-Pkl. 07.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 31 AUGUST 2025
-Pkl. 07.00 Wib,</t>
-  </si>
-  <si>
-    <t>DP/PA</t>
-  </si>
-  <si>
-    <t>W/PB</t>
-  </si>
-  <si>
-    <t>Persembahan</t>
-  </si>
-  <si>
-    <t>Multimedia</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>UMUM</t>
-  </si>
-  <si>
-    <t>REMAJA/PEMUDA</t>
-  </si>
-  <si>
-    <t>Majels Pendamping</t>
-  </si>
-  <si>
-    <t>Lektor 1</t>
-  </si>
-  <si>
-    <t>Lektor 2</t>
-  </si>
-  <si>
-    <t>Prokantor 1</t>
-  </si>
-  <si>
-    <t>Prokantor 2</t>
-  </si>
-  <si>
-    <t>Pemusik 1</t>
-  </si>
-  <si>
-    <t>Pemusik 2</t>
-  </si>
-  <si>
-    <t>Pemusik 3</t>
-  </si>
-  <si>
-    <t>Lektor 3</t>
-  </si>
-  <si>
-    <t>Prokantor 3</t>
-  </si>
-  <si>
-    <t>Lektor 4</t>
-  </si>
-  <si>
-    <t>P. Jemaat 1</t>
-  </si>
-  <si>
-    <t>P. Jemaat 2</t>
-  </si>
-  <si>
-    <t>P. Jemaat 3</t>
-  </si>
-  <si>
-    <t>P. Jemaat 4</t>
-  </si>
-  <si>
-    <t>Kolektan 1</t>
-  </si>
-  <si>
-    <t>Kolektan 2</t>
-  </si>
-  <si>
-    <t>Kolektan 4</t>
-  </si>
-  <si>
-    <t>Kolektan 3</t>
-  </si>
-  <si>
-    <t>MINGGU, 03 AUGUST 2025
-Pkl. 10.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 10 AUGUST 2025
-Pkl. 10.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 24 AUGUST 2025
-Pkl. 10.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 17 AUGUST 2025
-Pkl. 10.00 Wib,</t>
-  </si>
-  <si>
-    <t>MINGGU, 31 AUGUST 2025
+    <t>{Day}, {dd} {MMM} {yyyy}
 Pkl. 10.00 Wib,</t>
   </si>
 </sst>
@@ -543,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -563,24 +531,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -590,7 +558,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -600,7 +568,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -610,7 +578,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -620,7 +588,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -630,7 +598,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -640,7 +608,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -650,7 +618,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -660,7 +628,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -670,7 +638,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -680,7 +648,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -690,7 +658,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -700,7 +668,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -710,7 +678,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -720,7 +688,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -730,7 +698,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -740,7 +708,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -750,7 +718,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -760,7 +728,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -770,7 +738,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -780,7 +748,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -790,7 +758,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -808,7 +776,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -816,24 +784,24 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -843,7 +811,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>

</xml_diff>